<commit_message>
Pushing newer QDesc Jutsu
</commit_message>
<xml_diff>
--- a/Python Jutsu/Descriptive Results.xlsx
+++ b/Python Jutsu/Descriptive Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>count</t>
   </si>
@@ -49,10 +49,7 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Salary</t>
-  </si>
-  <si>
-    <t>Satisfaction</t>
+    <t>sleep(hrs)/weeknights</t>
   </si>
 </sst>
 </file>
@@ -384,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -427,31 +424,31 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>589</v>
+        <v>671</v>
       </c>
       <c r="C2">
-        <v>40.73</v>
+        <v>49.8</v>
       </c>
       <c r="D2">
-        <v>9.970000000000001</v>
+        <v>19.36</v>
       </c>
       <c r="E2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F2">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G2">
-        <v>13.34</v>
+        <v>25.2</v>
       </c>
       <c r="H2">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I2">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="J2">
-        <v>8.68</v>
+        <v>7.38</v>
       </c>
       <c r="K2">
         <v>0.01</v>
@@ -462,68 +459,33 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>589</v>
+        <v>671</v>
       </c>
       <c r="C3">
-        <v>39900.66</v>
+        <v>7.63</v>
       </c>
       <c r="D3">
-        <v>16511.58</v>
+        <v>1.39</v>
       </c>
       <c r="E3">
-        <v>39731</v>
+        <v>8.34</v>
       </c>
       <c r="F3">
-        <v>14795</v>
+        <v>0.98</v>
       </c>
       <c r="G3">
-        <v>21935.07</v>
+        <v>1.45</v>
       </c>
       <c r="H3">
-        <v>12027</v>
+        <v>4.52</v>
       </c>
       <c r="I3">
-        <v>67877</v>
+        <v>9.880000000000001</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>35.7</v>
       </c>
       <c r="K3">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>589</v>
-      </c>
-      <c r="C4">
-        <v>3.55</v>
-      </c>
-      <c r="D4">
-        <v>1.47</v>
-      </c>
-      <c r="E4">
-        <v>3.58</v>
-      </c>
-      <c r="F4">
-        <v>1.32</v>
-      </c>
-      <c r="G4">
-        <v>1.95</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>5.99</v>
-      </c>
-      <c r="J4">
-        <v>8.210000000000001</v>
-      </c>
-      <c r="K4">
         <v>0.01</v>
       </c>
     </row>

</xml_diff>